<commit_message>
hydroalt, fix cat variables
</commit_message>
<xml_diff>
--- a/r/xlsx/themes.xlsx
+++ b/r/xlsx/themes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeff/git/ecosheds/lmg-restore/r/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E63CB4CD-AEF5-B540-B258-69B2BB6EC0E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7704823D-87C4-BB4D-8B5F-47C8805C9827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51200" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="1" xr2:uid="{AE99D6E3-0A03-B54F-A17C-78F34962647F}"/>
+    <workbookView xWindow="-51200" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="2" xr2:uid="{AE99D6E3-0A03-B54F-A17C-78F34962647F}"/>
   </bookViews>
   <sheets>
     <sheet name="themes" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3562" uniqueCount="849">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3564" uniqueCount="850">
   <si>
     <t>theme</t>
   </si>
@@ -2494,9 +2494,6 @@
     <t>Probability streamflow exceeds a given value. The exceedance probability is used to calculate flow duration curves.</t>
   </si>
   <si>
-    <t>none</t>
-  </si>
-  <si>
     <t>pre</t>
   </si>
   <si>
@@ -2585,6 +2582,12 @@
   </si>
   <si>
     <t>Eco-Deficit</t>
+  </si>
+  <si>
+    <t>dims_exceedance</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -3003,10 +3006,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3299DF9C-F617-B646-BEE4-AB38FAC7FD15}">
-  <dimension ref="A1:O12"/>
+  <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView topLeftCell="F8" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView topLeftCell="A5" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3022,7 +3025,7 @@
     <col min="10" max="10" width="23.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>213</v>
       </c>
@@ -3060,16 +3063,19 @@
         <v>475</v>
       </c>
       <c r="M1" t="s">
+        <v>848</v>
+      </c>
+      <c r="N1" t="s">
         <v>266</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>267</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="119" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="119" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>214</v>
       </c>
@@ -3097,8 +3103,11 @@
       <c r="L2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" ht="85" x14ac:dyDescent="0.2">
+      <c r="M2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>214</v>
       </c>
@@ -3133,17 +3142,20 @@
       <c r="L3" t="b">
         <v>0</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="M3" t="b">
+        <v>0</v>
+      </c>
+      <c r="N3" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="N3">
-        <v>1</v>
-      </c>
-      <c r="O3" t="s">
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="68" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>214</v>
       </c>
@@ -3178,17 +3190,20 @@
       <c r="L4" t="b">
         <v>0</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="M4" t="b">
+        <v>0</v>
+      </c>
+      <c r="N4" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="N4">
-        <v>1</v>
-      </c>
-      <c r="O4" t="s">
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="P4" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="119" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" ht="119" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>214</v>
       </c>
@@ -3225,14 +3240,17 @@
       <c r="L5" t="b">
         <v>1</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="M5" t="b">
+        <v>0</v>
+      </c>
+      <c r="N5" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="136" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" ht="136" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>214</v>
       </c>
@@ -3267,8 +3285,11 @@
       <c r="L6" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" ht="85" x14ac:dyDescent="0.2">
+      <c r="M6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>214</v>
       </c>
@@ -3301,17 +3322,20 @@
       <c r="L7" t="b">
         <v>0</v>
       </c>
-      <c r="M7" t="s">
+      <c r="M7" t="b">
+        <v>0</v>
+      </c>
+      <c r="N7" t="s">
         <v>272</v>
       </c>
-      <c r="N7">
-        <v>1</v>
-      </c>
-      <c r="O7" t="s">
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="102" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>215</v>
       </c>
@@ -3342,8 +3366,11 @@
       <c r="L8" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" ht="85" x14ac:dyDescent="0.2">
+      <c r="M8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>215</v>
       </c>
@@ -3376,145 +3403,157 @@
       <c r="L9" t="b">
         <v>0</v>
       </c>
-      <c r="M9" t="s">
+      <c r="M9" t="b">
+        <v>0</v>
+      </c>
+      <c r="N9" t="s">
         <v>274</v>
       </c>
-      <c r="N9">
-        <v>1</v>
-      </c>
-      <c r="O9" t="s">
+      <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="P9" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="85" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" ht="170" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>215</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>10</v>
+        <v>809</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>472</v>
+        <v>810</v>
       </c>
       <c r="D10" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>719</v>
+        <v>811</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>328</v>
+        <v>812</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>329</v>
+        <v>813</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>18</v>
+        <v>215</v>
       </c>
       <c r="K10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L10" t="b">
         <v>0</v>
       </c>
-      <c r="M10" t="s">
-        <v>295</v>
-      </c>
-      <c r="N10">
-        <v>1</v>
-      </c>
-      <c r="O10" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" ht="85" x14ac:dyDescent="0.2">
+      <c r="M10" t="b">
+        <v>1</v>
+      </c>
+      <c r="N10" t="s">
+        <v>814</v>
+      </c>
+      <c r="O10">
+        <v>2</v>
+      </c>
+      <c r="P10" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>215</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>220</v>
+        <v>472</v>
       </c>
       <c r="D11" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
+      <c r="I11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="K11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L11" t="b">
         <v>0</v>
       </c>
-      <c r="M11" t="s">
-        <v>276</v>
-      </c>
-      <c r="N11">
-        <v>1</v>
-      </c>
-      <c r="O11" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" ht="170" x14ac:dyDescent="0.2">
+      <c r="M11" t="b">
+        <v>0</v>
+      </c>
+      <c r="N11" t="s">
+        <v>295</v>
+      </c>
+      <c r="O11">
+        <v>1</v>
+      </c>
+      <c r="P11" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>215</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>809</v>
+        <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>810</v>
+        <v>220</v>
       </c>
       <c r="D12" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>811</v>
+        <v>720</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>812</v>
+        <v>330</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>813</v>
+        <v>327</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>215</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
       <c r="K12" t="b">
         <v>0</v>
       </c>
       <c r="L12" t="b">
         <v>0</v>
       </c>
-      <c r="M12" t="s">
-        <v>814</v>
-      </c>
-      <c r="N12">
-        <v>2</v>
-      </c>
-      <c r="O12" t="s">
-        <v>815</v>
+      <c r="M12" t="b">
+        <v>0</v>
+      </c>
+      <c r="N12" t="s">
+        <v>276</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="P12" t="s">
+        <v>277</v>
       </c>
     </row>
   </sheetData>
@@ -3524,7 +3563,7 @@
     <hyperlink ref="G6" r:id="rId3" xr:uid="{2A6DFADB-88E1-5A48-96D8-44A804028C72}"/>
     <hyperlink ref="G7" r:id="rId4" xr:uid="{796C75A3-A990-CE43-9F4F-B9CF62A99DD8}"/>
     <hyperlink ref="G5" r:id="rId5" xr:uid="{CB3A387E-3E47-3544-8A79-337A24241FC9}"/>
-    <hyperlink ref="G12" r:id="rId6" xr:uid="{0999B51A-918A-E94F-97CE-572937D40B57}"/>
+    <hyperlink ref="G10" r:id="rId6" xr:uid="{0999B51A-918A-E94F-97CE-572937D40B57}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3534,9 +3573,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{356FD21B-BA3B-0140-999A-460BCE259E1F}">
   <dimension ref="A1:S222"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A159" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L220" sqref="L220"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A158" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N212" sqref="N212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15446,49 +15485,49 @@
         <v>810</v>
       </c>
       <c r="E214" t="s">
-        <v>816</v>
+        <v>818</v>
       </c>
       <c r="F214" t="s">
         <v>837</v>
       </c>
       <c r="G214" t="s">
-        <v>818</v>
+        <v>820</v>
       </c>
       <c r="H214" t="s">
-        <v>817</v>
+        <v>819</v>
       </c>
       <c r="I214" t="s">
         <v>35</v>
       </c>
       <c r="J214">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="K214">
-        <v>100</v>
+        <v>9100</v>
       </c>
       <c r="L214">
-        <v>0.03</v>
+        <v>1E-4</v>
       </c>
       <c r="M214">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="N214" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="O214" t="s">
-        <v>37</v>
+        <v>331</v>
       </c>
       <c r="P214" t="b">
         <v>1</v>
       </c>
       <c r="Q214" t="s">
-        <v>37</v>
+        <v>312</v>
       </c>
       <c r="R214" t="b">
         <v>1</v>
       </c>
       <c r="S214" t="s">
-        <v>37</v>
+        <v>312</v>
       </c>
     </row>
     <row r="215" spans="1:19" x14ac:dyDescent="0.2">
@@ -15505,16 +15544,16 @@
         <v>810</v>
       </c>
       <c r="E215" t="s">
-        <v>819</v>
+        <v>821</v>
       </c>
       <c r="F215" t="s">
         <v>838</v>
       </c>
       <c r="G215" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="H215" t="s">
-        <v>820</v>
+        <v>822</v>
       </c>
       <c r="I215" t="s">
         <v>35</v>
@@ -15523,13 +15562,13 @@
         <v>0</v>
       </c>
       <c r="K215">
-        <v>9100</v>
+        <v>15500</v>
       </c>
       <c r="L215">
         <v>1E-4</v>
       </c>
       <c r="M215">
-        <v>1000</v>
+        <v>100000</v>
       </c>
       <c r="N215" t="s">
         <v>36</v>
@@ -15564,49 +15603,22 @@
         <v>810</v>
       </c>
       <c r="E216" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c r="F216" t="s">
         <v>839</v>
       </c>
-      <c r="G216" t="s">
-        <v>821</v>
-      </c>
       <c r="H216" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
       <c r="I216" t="s">
-        <v>35</v>
-      </c>
-      <c r="J216">
-        <v>0</v>
-      </c>
-      <c r="K216">
-        <v>15500</v>
-      </c>
-      <c r="L216">
-        <v>1E-4</v>
-      </c>
-      <c r="M216">
-        <v>100000</v>
-      </c>
-      <c r="N216" t="s">
-        <v>36</v>
-      </c>
-      <c r="O216" t="s">
-        <v>331</v>
+        <v>72</v>
       </c>
       <c r="P216" t="b">
         <v>1</v>
       </c>
-      <c r="Q216" t="s">
-        <v>312</v>
-      </c>
       <c r="R216" t="b">
         <v>1</v>
-      </c>
-      <c r="S216" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="217" spans="1:19" x14ac:dyDescent="0.2">
@@ -15623,16 +15635,49 @@
         <v>810</v>
       </c>
       <c r="E217" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="F217" t="s">
         <v>840</v>
       </c>
+      <c r="G217" t="s">
+        <v>827</v>
+      </c>
       <c r="H217" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="I217" t="s">
-        <v>72</v>
+        <v>35</v>
+      </c>
+      <c r="J217">
+        <v>0</v>
+      </c>
+      <c r="K217">
+        <v>18700</v>
+      </c>
+      <c r="L217">
+        <v>1E-4</v>
+      </c>
+      <c r="M217">
+        <v>10000</v>
+      </c>
+      <c r="N217" t="s">
+        <v>36</v>
+      </c>
+      <c r="O217" t="s">
+        <v>331</v>
+      </c>
+      <c r="P217" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q217" t="s">
+        <v>312</v>
+      </c>
+      <c r="R217" t="b">
+        <v>1</v>
+      </c>
+      <c r="S217" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="218" spans="1:19" x14ac:dyDescent="0.2">
@@ -15649,16 +15694,16 @@
         <v>810</v>
       </c>
       <c r="E218" t="s">
-        <v>826</v>
+        <v>828</v>
       </c>
       <c r="F218" t="s">
         <v>841</v>
       </c>
       <c r="G218" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="H218" t="s">
-        <v>827</v>
+        <v>829</v>
       </c>
       <c r="I218" t="s">
         <v>35</v>
@@ -15667,7 +15712,7 @@
         <v>0</v>
       </c>
       <c r="K218">
-        <v>18700</v>
+        <v>18000</v>
       </c>
       <c r="L218">
         <v>1E-4</v>
@@ -15708,49 +15753,49 @@
         <v>810</v>
       </c>
       <c r="E219" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="F219" t="s">
         <v>842</v>
       </c>
       <c r="G219" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="H219" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="I219" t="s">
         <v>35</v>
       </c>
       <c r="J219">
-        <v>0</v>
+        <v>-500</v>
       </c>
       <c r="K219">
-        <v>18000</v>
+        <v>6700</v>
       </c>
       <c r="L219">
-        <v>1E-4</v>
+        <v>-1</v>
       </c>
       <c r="M219">
-        <v>10000</v>
+        <v>500</v>
       </c>
       <c r="N219" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="O219" t="s">
-        <v>331</v>
+        <v>37</v>
       </c>
       <c r="P219" t="b">
         <v>1</v>
       </c>
       <c r="Q219" t="s">
-        <v>312</v>
+        <v>37</v>
       </c>
       <c r="R219" t="b">
         <v>1</v>
       </c>
       <c r="S219" t="s">
-        <v>312</v>
+        <v>37</v>
       </c>
     </row>
     <row r="220" spans="1:19" x14ac:dyDescent="0.2">
@@ -15767,31 +15812,28 @@
         <v>810</v>
       </c>
       <c r="E220" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="F220" t="s">
-        <v>843</v>
-      </c>
-      <c r="G220" t="s">
-        <v>828</v>
+        <v>844</v>
       </c>
       <c r="H220" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="I220" t="s">
         <v>35</v>
       </c>
       <c r="J220">
-        <v>-500</v>
+        <v>-5.1700000000000003E-2</v>
       </c>
       <c r="K220">
-        <v>6700</v>
+        <v>2.8969999999999998</v>
       </c>
       <c r="L220">
-        <v>-500</v>
+        <v>0</v>
       </c>
       <c r="M220">
-        <v>6700</v>
+        <v>3</v>
       </c>
       <c r="N220" t="s">
         <v>42</v>
@@ -15826,28 +15868,25 @@
         <v>810</v>
       </c>
       <c r="E221" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="F221" t="s">
-        <v>845</v>
-      </c>
-      <c r="G221" t="s">
-        <v>818</v>
+        <v>843</v>
       </c>
       <c r="H221" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="I221" t="s">
         <v>35</v>
       </c>
       <c r="J221">
-        <v>-5.1700000000000003E-2</v>
+        <v>-0.54657999999999995</v>
       </c>
       <c r="K221">
-        <v>2.8969999999999998</v>
+        <v>2.8970199999999999</v>
       </c>
       <c r="L221">
-        <v>-0.1</v>
+        <v>0</v>
       </c>
       <c r="M221">
         <v>3</v>
@@ -15885,31 +15924,28 @@
         <v>810</v>
       </c>
       <c r="E222" t="s">
-        <v>835</v>
+        <v>816</v>
       </c>
       <c r="F222" t="s">
-        <v>844</v>
-      </c>
-      <c r="G222" t="s">
-        <v>818</v>
+        <v>836</v>
       </c>
       <c r="H222" t="s">
-        <v>836</v>
+        <v>817</v>
       </c>
       <c r="I222" t="s">
         <v>35</v>
       </c>
       <c r="J222">
-        <v>-0.54657999999999995</v>
+        <v>0.03</v>
       </c>
       <c r="K222">
-        <v>2.8970199999999999</v>
+        <v>100</v>
       </c>
       <c r="L222">
-        <v>-0.6</v>
+        <v>0</v>
       </c>
       <c r="M222">
-        <v>3</v>
+        <v>100</v>
       </c>
       <c r="N222" t="s">
         <v>42</v>
@@ -15918,13 +15954,13 @@
         <v>37</v>
       </c>
       <c r="P222" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q222" t="s">
         <v>37</v>
       </c>
       <c r="R222" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S222" t="s">
         <v>37</v>
@@ -15939,10 +15975,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{987CF23D-DD6E-FA4F-ABEA-A0891733CE0A}">
-  <dimension ref="A1:D285"/>
+  <dimension ref="A1:D286"/>
   <sheetViews>
-    <sheetView topLeftCell="A214" workbookViewId="0">
-      <selection activeCell="A285" sqref="A285"/>
+    <sheetView tabSelected="1" topLeftCell="A215" workbookViewId="0">
+      <selection activeCell="D286" sqref="D286"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19918,13 +19954,13 @@
         <v>809</v>
       </c>
       <c r="B284" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="C284" t="s">
+        <v>845</v>
+      </c>
+      <c r="D284" t="s">
         <v>846</v>
-      </c>
-      <c r="D284" t="s">
-        <v>847</v>
       </c>
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.2">
@@ -19932,13 +19968,27 @@
         <v>809</v>
       </c>
       <c r="B285" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="C285" t="s">
         <v>621</v>
       </c>
       <c r="D285" t="s">
-        <v>848</v>
+        <v>847</v>
+      </c>
+    </row>
+    <row r="286" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A286" t="s">
+        <v>809</v>
+      </c>
+      <c r="B286" t="s">
+        <v>823</v>
+      </c>
+      <c r="C286" t="s">
+        <v>849</v>
+      </c>
+      <c r="D286" t="s">
+        <v>849</v>
       </c>
     </row>
   </sheetData>

</xml_diff>